<commit_message>
Update Check Ve TBD
</commit_message>
<xml_diff>
--- a/document/TestCaseAsign.xlsx
+++ b/document/TestCaseAsign.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E0C4B-E980-4AD2-9DCE-40876F6E07D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Đức</t>
   </si>
@@ -94,12 +95,27 @@
   </si>
   <si>
     <t>Student</t>
+  </si>
+  <si>
+    <t>Kiểm tra link Về TDB</t>
+  </si>
+  <si>
+    <t>Check Về TBD</t>
+  </si>
+  <si>
+    <t>baseURL: https://tbd.edu.vn/</t>
+  </si>
+  <si>
+    <t>Text của h1.titleMainPage</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,20 +426,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -521,6 +538,29 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Update Check Ve TBD"
</commit_message>
<xml_diff>
--- a/document/TestCaseAsign.xlsx
+++ b/document/TestCaseAsign.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E0C4B-E980-4AD2-9DCE-40876F6E07D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Đức</t>
   </si>
@@ -95,27 +94,12 @@
   </si>
   <si>
     <t>Student</t>
-  </si>
-  <si>
-    <t>Kiểm tra link Về TDB</t>
-  </si>
-  <si>
-    <t>Check Về TBD</t>
-  </si>
-  <si>
-    <t>baseURL: https://tbd.edu.vn/</t>
-  </si>
-  <si>
-    <t>Text của h1.titleMainPage</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,21 +410,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -538,29 +521,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
D Tuan check Daotao
</commit_message>
<xml_diff>
--- a/document/TestCaseAsign.xlsx
+++ b/document/TestCaseAsign.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E0C4B-E980-4AD2-9DCE-40876F6E07D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B5B931-9C38-4924-8D11-FF7F7080EEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4368" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Đức</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Check Đào tạo</t>
+  </si>
+  <si>
+    <t>WebElement: https://tbd.edu.vn/dao-tao/</t>
+  </si>
+  <si>
+    <t>Test Link Passed!</t>
+  </si>
+  <si>
+    <t>Đào tạo</t>
   </si>
 </sst>
 </file>
@@ -427,23 +439,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -459,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -467,7 +480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -475,7 +488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -483,7 +496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -491,7 +504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -499,7 +512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -507,7 +520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -515,7 +528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -538,7 +551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -559,6 +572,29 @@
       </c>
       <c r="G12" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xuân hồng check nghiên cứu
</commit_message>
<xml_diff>
--- a/document/TestCaseAsign.xlsx
+++ b/document/TestCaseAsign.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B5B931-9C38-4924-8D11-FF7F7080EEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B742AD00-6E3D-4E82-BF09-449A22EDBACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4368" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Đức</t>
   </si>
@@ -122,6 +122,21 @@
   </si>
   <si>
     <t>Đào tạo</t>
+  </si>
+  <si>
+    <t>Check Nghiên cứu</t>
+  </si>
+  <si>
+    <t>Kiểm tra link Về TDB</t>
+  </si>
+  <si>
+    <t>WebElement: https://tbd.edu.vn/nghien-cuu/</t>
+  </si>
+  <si>
+    <t>Nghiên cứu</t>
+  </si>
+  <si>
+    <t>Xuân Hồng</t>
   </si>
 </sst>
 </file>
@@ -439,24 +454,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -472,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -480,7 +495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -488,7 +503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -496,7 +511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -504,7 +519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -512,7 +527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -520,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -528,7 +543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -551,7 +566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -574,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -595,6 +610,29 @@
       </c>
       <c r="G13" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update sinh vien link
</commit_message>
<xml_diff>
--- a/document/TestCaseAsign.xlsx
+++ b/document/TestCaseAsign.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{B742AD00-6E3D-4E82-BF09-449A22EDBACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AEB370D-1F4A-4B5D-B188-A4B7F938C3E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59AFD16-215D-466D-902E-3F47D97AD54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Đức</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>WebElement: https://tbd.edu.vn/tuyen-sinh/</t>
+  </si>
+  <si>
+    <t>Check Sinh viên</t>
+  </si>
+  <si>
+    <t>WebElement: https://tbd.edu.vn/sinh-vien/</t>
   </si>
 </sst>
 </file>
@@ -460,24 +466,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -493,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -501,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -509,7 +515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -517,7 +523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -525,7 +531,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -533,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -541,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -549,7 +555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -572,7 +578,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -595,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -618,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -641,7 +647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -662,6 +668,29 @@
       </c>
       <c r="G15" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Added drive edge and test case login
</commit_message>
<xml_diff>
--- a/document/TestCaseAsign.xlsx
+++ b/document/TestCaseAsign.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Đức</t>
   </si>
@@ -192,19 +192,41 @@
   </si>
   <si>
     <t>Tittle: Tra cứu hồ sơ-Đại học Thái Bình Dương</t>
+  </si>
+  <si>
+    <t>Login 2</t>
+  </si>
+  <si>
+    <t>1. Open site https://daotao.tbd.edu.vn
+2. Enter username/password</t>
+  </si>
+  <si>
+    <t>Check login for daotao.tbd.edu.vn fail case</t>
+  </si>
+  <si>
+    <t>username/password : 225282478/empty</t>
+  </si>
+  <si>
+    <t>Tên đăng nhập và mật khẩu không hợp lệ, bạn nhập lại !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA94442"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,11 +249,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,16 +535,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="43.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
@@ -795,6 +818,32 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>